<commit_message>
Protege celdas a valores incorrectos
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -271,18 +271,18 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -428,85 +428,9 @@
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="20">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D4" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D5" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E3" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E5" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F3" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F5" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G3" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G4" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G5" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6" type="list">
-      <formula1>"v1,v2,v3"</formula1>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D1:G6" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>